<commit_message>
Refactor article normalization and header detection in price parser
</commit_message>
<xml_diff>
--- a/resapolon.xlsx
+++ b/resapolon.xlsx
@@ -536,12 +536,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3512010-</t>
+          <t>11.3512010-</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3512010</t>
+          <t>113512010</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -780,28 +780,36 @@
           <t>У.036.57.000-02- | Муфта разрывная КОМПЛЕКТ М 16/22х1,5 пневмошлангов прицепа в ком-кте с переходником (ком-т, ЖЕЛТЫЙ)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16/22Х1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1622Х1</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>С 075195-СПЕЦМАШ</t>
+          <t>D-16мм-СПЕЦМАШ</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Пневмогидроэлемент МАЗ подрессоривания сидения</t>
+          <t>Трубка полиамидная, тормозная (D=16 мм) в бухте 50 м.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>075195ССПЕЦМАШ</t>
+          <t>16ММDСПЕЦМАШ</t>
         </is>
       </c>
       <c r="G9" t="n">
         <v>85.5</v>
       </c>
       <c r="H9" t="n">
-        <v>3295</v>
+        <v>129</v>
       </c>
       <c r="I9" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Implement structural updates and optimizations across multiple modules
</commit_message>
<xml_diff>
--- a/resapolon.xlsx
+++ b/resapolon.xlsx
@@ -529,84 +529,84 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>11.3512010- | Регулятор давления воздуха ЗИЛ, МАЗ, УРАЛ, КРАЗ, ЛИАЗ</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>11.3512010-</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>113512010</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>100-3512010-СПЕЦМАШ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>11.3512010-СПЕЦМАШ</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Регулятор давления воздуха ЗИЛ, МАЗ, УРАЛ, КРАЗ, ЛИАЗ</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1003512010СПЕЦМАШ</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>95</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1695</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>113512010СПЕЦМАШ</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1375</v>
+      </c>
+      <c r="I3" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>1200-20- | Лента ободная (ФЛИППЕР) широкая 1200-20 для автокамеры 300-320 (упак. 10 шт)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1200-20-</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1200-20</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>120020</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1200-20-СПЕЦМАШ</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Лента ободная (ФЛИППЕР) ширина = 230 мм, 1200-20 для автокамеры</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>120020СПЕЦМАШ</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>80.1834862385321</v>
-      </c>
-      <c r="H4" t="n">
-        <v>875</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>1200-24-СПЕЦМАШ</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Лента ободная (ФЛИППЕР) ширина = 220 мм, 1200-24 для автокамеры 325/95 R 24</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>120024СПЕЦМАШ</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1095</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <v>4</v>
       </c>
     </row>
@@ -652,84 +652,84 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>238-1308012-А4- | Крыльчатка вентилятора внутр Dвн.-50 мм (ПОЛИАМИД укрепл.с/вол. раб.темп. -50 +120 Профиль 4Н)</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>238-1308012-А4-</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>1308012238А4</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>238-1308012-А4-СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Крыльчатка вентилятора внутр Dвн.-50 мм (ПОЛИАМИД укрепл.с/вол. раб.темп. -50 +120 Профиль 4Н)</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>1308012238А4СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>95</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="G6" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2" t="n">
         <v>1375</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>100-3514008- | Кран тормозной главный, 100-3514008</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>100-3514008-</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>1003514008</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>100-3514008-СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Кран тормозной главный, 100-3514008</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>1003514008СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>95</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="G7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>2995</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -816,84 +816,84 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>5432-2402052- | Манжета (85х110-1,2) хвостовика редуктора (ФТОРСИЛИКОН) в упаковке</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>5432-2402052-</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>24020525432</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>5432-2402052-СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>Манжета (85х110-1,2) хвостовика редуктора (ФТОРСИЛИКОН) в упаковке</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>24020525432СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>95</v>
-      </c>
-      <c r="H10" t="n">
+      <c r="G10" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H10" s="2" t="n">
         <v>375</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>961-3519500- | Камера тормозная задняя (энергоаккумулятор ТИП-24/24 ДИСКОВЫХ ТОРМОЗОВ) 5490 (КОМ 925 481 430 0-СМ)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>961-3519500-</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>3519500961</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>961-3519500-СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Камера тормозная задняя (энергоаккумулятор ТИП-24/24 ДИСКОВЫХ ТОРМОЗОВ) 5490</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>3519500961СПЕЦМАШ</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>90</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="G11" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>5485</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>